<commit_message>
Refactoring of backtester, moving backtests into separate modules.
</commit_message>
<xml_diff>
--- a/backtester/test/calculations.xlsx
+++ b/backtester/test/calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-35200" yWindow="4720" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>10</v>
       </c>
@@ -494,7 +494,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>15</v>
       </c>
@@ -518,7 +518,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>17.5</v>
       </c>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:F12" si="2">A4*C4+E3</f>
+        <f t="shared" ref="E4:E11" si="2">A4*C4+E3</f>
         <v>15</v>
       </c>
       <c r="F4">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>12.5</v>
       </c>
@@ -565,15 +565,15 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="e">
+      <c r="K5" t="e">
         <f>AVERAGE(G2:G11)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>7.5</v>
       </c>
@@ -596,15 +596,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="2" t="e">
+      <c r="K6" s="2" t="e">
         <f>STDEVP(G2:G11)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>10</v>
       </c>
@@ -628,7 +628,7 @@
         <v>-0.36363636363636365</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>15</v>
       </c>
@@ -651,15 +651,15 @@
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="J8" t="e">
-        <f>SQRT(252)*J5/J6</f>
+      <c r="K8" t="e">
+        <f>SQRT(252)*K5/K6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>20</v>
       </c>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>22.5</v>
       </c>
@@ -707,7 +707,7 @@
         <v>-0.69230769230769229</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>17.5</v>
       </c>
@@ -730,36 +730,36 @@
         <f t="shared" si="0"/>
         <v>-1.75</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>4</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f>AVERAGE(E2:E11)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="D12" s="1"/>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>5</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f>STDEV(E2:E11)</f>
         <v>13.529802495068269</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="J13">
-        <f>J11/J12</f>
+    <row r="13" spans="1:11">
+      <c r="K13">
+        <f>K11/K12</f>
         <v>1.2564854517423036</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="I14" t="s">
+    <row r="14" spans="1:11">
+      <c r="J14" t="s">
         <v>6</v>
       </c>
-      <c r="J14">
-        <f>SQRT(252)*J11/J12</f>
+      <c r="K14">
+        <f>SQRT(252)*K11/K12</f>
         <v>19.946088187684705</v>
       </c>
     </row>

</xml_diff>